<commit_message>
Scripting SCD0335 until SCD0337
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0335 - Normal Skenario Admin SLN mengakses Report Log Pengiriman WA pada Digisales Portal.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0335 - Normal Skenario Admin SLN mengakses Report Log Pengiriman WA pada Digisales Portal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D3AC5F-187F-478E-B311-8759786E6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C4F237-12C5-4800-9150-1E28863644AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>